<commit_message>
changed source data , indicator and series files
</commit_message>
<xml_diff>
--- a/master_data/MINSET_series_catalog.xlsx
+++ b/master_data/MINSET_series_catalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\gender_data_portal\master_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FF8951F-C822-4D2A-8DF4-9446D758FAF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE7E6B6B-ED80-436B-B271-1D1B4F8A3ABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{976689F7-C737-417F-8155-A74B38AFF759}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{F1573CD7-C78D-4A08-B5EC-97AACCC03628}"/>
   </bookViews>
   <sheets>
     <sheet name="CL_SERIES" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CL_SERIES!$D$1:$F$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CL_SERIES!$D$1:$F$101</definedName>
     <definedName name="BigNum">9.99E+307</definedName>
     <definedName name="BigStr">REPT("z",255)</definedName>
     <definedName name="CauseOfDeath">#REF!</definedName>
@@ -55,7 +55,7 @@
     <definedName name="ReportMonth">IF(MonthName="",TEXT(MONTH(TODAY()),"mmm"),MonthName)</definedName>
     <definedName name="ReportYear">IF(Year="",YEAR(TODAY()),Year)</definedName>
     <definedName name="ScheduleHighlight">#REF!</definedName>
-    <definedName name="Series">CL_SERIES!$D$1:$F$71</definedName>
+    <definedName name="Series">CL_SERIES!$D$1:$F$73</definedName>
     <definedName name="Sex">[1]CL_SEX!#REF!</definedName>
     <definedName name="Start_time">#REF!</definedName>
     <definedName name="TimesList">#REF!</definedName>
@@ -83,15 +83,60 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={A1D8E90B-F54A-4D78-85F7-1A10ABA461CE}</author>
+    <author>tc={E5ED01E1-972C-408A-A7CB-22BFC0D4D8C2}</author>
+    <author>tc={C79C9CCA-207C-4FFC-B12D-49A4EAB86B66}</author>
+    <author>tc={D3A3F677-F5E9-4154-937E-2559F3B1C349}</author>
+    <author>tc={95D651FE-A347-4461-995C-6037E9D8318F}</author>
+    <author>tc={5C257CF8-1145-4CBB-BCED-54A1A43F1313}</author>
+    <author>tc={723DCC6B-7081-4C10-BF1E-7D7D3F6F467B}</author>
   </authors>
   <commentList>
-    <comment ref="H37" authorId="0" shapeId="0" xr:uid="{A1D8E90B-F54A-4D78-85F7-1A10ABA461CE}">
+    <comment ref="E29" authorId="0" shapeId="0" xr:uid="{E5ED01E1-972C-408A-A7CB-22BFC0D4D8C2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Gross graduation ratio from tertiary education</t>
+    Can be approximated by the total net enrolment rate: http://data.uis.unesco.org/index.aspx?queryid=3813</t>
+      </text>
+    </comment>
+    <comment ref="E35" authorId="1" shapeId="0" xr:uid="{C79C9CCA-207C-4FFC-B12D-49A4EAB86B66}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    No longer available</t>
+      </text>
+    </comment>
+    <comment ref="E37" authorId="2" shapeId="0" xr:uid="{D3A3F677-F5E9-4154-937E-2559F3B1C349}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    No longer available</t>
+      </text>
+    </comment>
+    <comment ref="E38" authorId="3" shapeId="0" xr:uid="{95D651FE-A347-4461-995C-6037E9D8318F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    No longer available. The UIS called this indicator “gross intake ratio to last grade”. The completion rate (CR_1, CR_1_F, CF_1_M) is a related but different indicator.</t>
+      </text>
+    </comment>
+    <comment ref="E39" authorId="4" shapeId="0" xr:uid="{5C257CF8-1145-4CBB-BCED-54A1A43F1313}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    No longer available. The UIS called this indicator “gross intake ratio to last grade”. The completion rate (CR_1, CR_1_F, CF_1_M) is a related but different indicator.</t>
+      </text>
+    </comment>
+    <comment ref="E40" authorId="5" shapeId="0" xr:uid="{723DCC6B-7081-4C10-BF1E-7D7D3F6F467B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    No longer available. The UIS called this indicator “gross intake ratio to last grade”. The completion rate (CR_1, CR_1_F, CF_1_M) is a related but different indicator.</t>
       </text>
     </comment>
   </commentList>
@@ -99,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="172">
   <si>
     <t>INDICATOR_ID</t>
   </si>
@@ -131,6 +176,9 @@
     <t>Tags</t>
   </si>
   <si>
+    <t>Comment</t>
+  </si>
+  <si>
     <t>Average number of hours spent on domestic chores and care work, by sex, age and location</t>
   </si>
   <si>
@@ -173,7 +221,7 @@
     <t>Proportion of employed who are own-account workers, by sex</t>
   </si>
   <si>
-    <t>EMP_TEMP_SEX_STE_DT_A</t>
+    <t>EMP_2EMP_SEX_STE_NB_A</t>
   </si>
   <si>
     <t>Proportion of employed who are contributing family workers, by sex</t>
@@ -188,7 +236,7 @@
     <t>Percentage distribution of employed population in agricultural sector, by sex</t>
   </si>
   <si>
-    <t>EMP_TEMP_SEX_ECO_DT_A</t>
+    <t>EMP_TEMP_SEX_ECO_NB_A</t>
   </si>
   <si>
     <t>economy, employment</t>
@@ -209,7 +257,19 @@
     <t>Unemployment rate, by sex, age and persons with disabilities</t>
   </si>
   <si>
-    <t>SL_TLF_UEM; SL_TLF_UEMDIS</t>
+    <t>SL_TLF_UEM</t>
+  </si>
+  <si>
+    <t>changed into 108 "'Unemployment rate, by sex and age"</t>
+  </si>
+  <si>
+    <t>Unemployment rate, by sex and age</t>
+  </si>
+  <si>
+    <t>Unemployment rate, by sex and disability</t>
+  </si>
+  <si>
+    <t>SL_TLF_UEMDIS</t>
   </si>
   <si>
     <t>Proportion of adults (15 years and older) with an account at a bank or other financial institution or with a mobile-money-service provider, by sex</t>
@@ -257,16 +317,7 @@
     <t>Youth literacy rate of persons (15-24 years), by sex</t>
   </si>
   <si>
-    <r>
-      <t>LR_Ag15t24, LR_Ag15t24_F, LR_Ag15t24_M, LR_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="MS Sans Serif"/>
-      </rPr>
-      <t>Ag15t24_gpia</t>
-    </r>
+    <t>LR_Ag15t24, LR_Ag15t24_F, LR_Ag15t24_M, LR_Ag15t24_gpia</t>
   </si>
   <si>
     <t>Education</t>
@@ -278,9 +329,6 @@
     <t>Adjusted net enrolment rate in primary education by sex</t>
   </si>
   <si>
-    <t>NERA_1_cp, NERA_1_F_cp, NERA_1_M_cp, NERA_1_gpi</t>
-  </si>
-  <si>
     <t>Gross enrolment ratio in secondary education, by sex</t>
   </si>
   <si>
@@ -314,9 +362,6 @@
     <t>Share of female science, technology, engineering and mathematics graduates at tertiary level</t>
   </si>
   <si>
-    <t>FGP_5T8_F500600700</t>
-  </si>
-  <si>
     <t>education, youth</t>
   </si>
   <si>
@@ -329,35 +374,13 @@
     <t>Adjusted net intake rate to the first grade of primary education, by sex</t>
   </si>
   <si>
-    <t>NIRA_1_cp, NIRA_1_F_cp, NIRA_1_M_cp, NIRA_1_gpi</t>
-  </si>
-  <si>
     <t>Primary education completion rate (proxy), by sex</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">CR_1, CR_1_F, CF_1_M, </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="10"/>
-        <rFont val="MS Sans Serif"/>
-      </rPr>
-      <t>AIR_1_Glast, AIR_1_Glast_F, AIR_1_Glast_M, AIR_1_Glast_gpi</t>
-    </r>
-  </si>
-  <si>
     <t>Gross graduation ratio from lower secondary education, by sex</t>
   </si>
   <si>
-    <t>GGR_2, GGR_2_F, GGR_2_M, GGR_2_gpi</t>
-  </si>
-  <si>
     <t>Effective transition rate from primary to secondary education (general programmes), by sex</t>
-  </si>
-  <si>
-    <t>TRANRA_2_GPV_CP, TRANRA_2_GPV_F_CP, TRANRA_2_GPV_M_CP, TRANRA_2_GPV_GPI</t>
   </si>
   <si>
     <t>Educational attainment (minimum lower secondary) of the population aged 25 and older, by sex</t>
@@ -643,11 +666,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="10"/>
-      <name val="MS Sans Serif"/>
-    </font>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -661,7 +680,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -705,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -722,22 +741,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -780,7 +796,7 @@
         <xdr:cNvPr id="2" name="EsriDoNotEdit">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFCCB341-7F59-40C7-A0E2-E7BA9A8B74C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D8518A5-3B8E-46E8-9BA3-1E5E701A3298}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -871,6 +887,7 @@
       <sheetName val="FuzzyLookup_AddIn_Undo_Sheet"/>
       <sheetName val="CL_COD_old"/>
       <sheetName val="CL_COD"/>
+      <sheetName val="CL_DISABILITY"/>
       <sheetName val="CL_EDU_LEVEL"/>
       <sheetName val="CL_INDICATORS"/>
       <sheetName val="CL_METADATA_CATEGORY"/>
@@ -906,6 +923,7 @@
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
       <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -913,7 +931,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Lingyan Hu" id="{A8AA9BBC-37FB-47EC-ABCC-A6F7574CC1AF}" userId="S::hu2@un.org::59b260a8-334d-46b7-b76f-561ce9fdb1fd" providerId="AD"/>
+  <person displayName="Lingyan Hu" id="{217E1CF4-7E58-4EA0-B35E-F26CDD0E0674}" userId="S::hu2@un.org::59b260a8-334d-46b7-b76f-561ce9fdb1fd" providerId="AD"/>
 </personList>
 </file>
 
@@ -1214,21 +1232,36 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="H37" dT="2021-05-13T14:48:42.49" personId="{A8AA9BBC-37FB-47EC-ABCC-A6F7574CC1AF}" id="{A1D8E90B-F54A-4D78-85F7-1A10ABA461CE}">
-    <text>Gross graduation ratio from tertiary education</text>
+  <threadedComment ref="E29" dT="2021-05-24T18:05:57.31" personId="{217E1CF4-7E58-4EA0-B35E-F26CDD0E0674}" id="{E5ED01E1-972C-408A-A7CB-22BFC0D4D8C2}">
+    <text>Can be approximated by the total net enrolment rate: http://data.uis.unesco.org/index.aspx?queryid=3813</text>
+  </threadedComment>
+  <threadedComment ref="E35" dT="2021-05-24T19:11:29.36" personId="{217E1CF4-7E58-4EA0-B35E-F26CDD0E0674}" id="{C79C9CCA-207C-4FFC-B12D-49A4EAB86B66}">
+    <text>No longer available</text>
+  </threadedComment>
+  <threadedComment ref="E37" dT="2021-05-24T19:11:29.36" personId="{217E1CF4-7E58-4EA0-B35E-F26CDD0E0674}" id="{D3A3F677-F5E9-4154-937E-2559F3B1C349}">
+    <text>No longer available</text>
+  </threadedComment>
+  <threadedComment ref="E38" dT="2021-05-24T19:15:33.14" personId="{217E1CF4-7E58-4EA0-B35E-F26CDD0E0674}" id="{95D651FE-A347-4461-995C-6037E9D8318F}">
+    <text>No longer available. The UIS called this indicator “gross intake ratio to last grade”. The completion rate (CR_1, CR_1_F, CF_1_M) is a related but different indicator.</text>
+  </threadedComment>
+  <threadedComment ref="E39" dT="2021-05-24T19:15:33.14" personId="{217E1CF4-7E58-4EA0-B35E-F26CDD0E0674}" id="{5C257CF8-1145-4CBB-BCED-54A1A43F1313}">
+    <text>No longer available. The UIS called this indicator “gross intake ratio to last grade”. The completion rate (CR_1, CR_1_F, CF_1_M) is a related but different indicator.</text>
+  </threadedComment>
+  <threadedComment ref="E40" dT="2021-05-24T19:15:33.14" personId="{217E1CF4-7E58-4EA0-B35E-F26CDD0E0674}" id="{723DCC6B-7081-4C10-BF1E-7D7D3F6F467B}">
+    <text>No longer available. The UIS called this indicator “gross intake ratio to last grade”. The completion rate (CR_1, CR_1_F, CF_1_M) is a related but different indicator.</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F49A59-33D5-4788-8CE8-A6E208014523}">
-  <dimension ref="A1:J99"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{579AC289-89EF-44AA-9D57-7C1C42EE71ED}">
+  <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="J8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1237,7 +1270,7 @@
     <col min="3" max="3" width="12.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="12" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="11" customWidth="1"/>
     <col min="7" max="7" width="28" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="86.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.140625" style="5" bestFit="1" customWidth="1"/>
@@ -1245,7 +1278,7 @@
     <col min="11" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1276,8 +1309,11 @@
       <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1291,19 +1327,19 @@
         <v>72</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1317,19 +1353,19 @@
         <v>87</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1343,19 +1379,19 @@
         <v>88</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1369,17 +1405,17 @@
         <v>73</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="3"/>
       <c r="I5" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1393,20 +1429,20 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1420,20 +1456,20 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -1447,20 +1483,20 @@
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="4" t="s">
-        <v>24</v>
+      <c r="G8" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -1474,20 +1510,20 @@
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="I9" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -1501,20 +1537,20 @@
         <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3"/>
-      <c r="G10" s="4" t="s">
-        <v>24</v>
+      <c r="G10" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -1528,14 +1564,14 @@
         <v>79</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F11" s="3"/>
       <c r="I11" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -1549,20 +1585,20 @@
         <v>6</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F12" s="3"/>
-      <c r="G12" s="4" t="s">
-        <v>29</v>
+      <c r="G12" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -1576,20 +1612,20 @@
         <v>7</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -1603,20 +1639,20 @@
         <v>8</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="4" t="s">
-        <v>29</v>
+      <c r="G14" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -1630,19 +1666,19 @@
         <v>74</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>10</v>
       </c>
@@ -1650,348 +1686,340 @@
         <v>10</v>
       </c>
       <c r="C16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2">
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
       </c>
       <c r="D17" s="2">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
       </c>
       <c r="D18" s="2">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="I18" s="5" t="s">
-        <v>12</v>
+      <c r="F18" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>80</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="1">
+      <c r="J19" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2">
+        <v>81</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="I20" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="2">
-        <v>82</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>14</v>
-      </c>
-      <c r="B20" s="1">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0</v>
-      </c>
-      <c r="D20" s="2">
-        <v>10</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" s="1">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
       </c>
       <c r="D21" s="2">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="I21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
       </c>
       <c r="D22" s="2">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F22" s="3"/>
+      <c r="G22" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="I22" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
       </c>
       <c r="D23" s="2">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F23" s="3"/>
       <c r="I23" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B24" s="1">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
       </c>
       <c r="D24" s="2">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="F24" s="3"/>
       <c r="I24" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B25" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
       </c>
       <c r="D25" s="2">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F25" s="3"/>
       <c r="I25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1">
+        <v>18</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>20</v>
-      </c>
-      <c r="B26" s="1">
-        <v>20</v>
-      </c>
-      <c r="C26" s="1">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2">
+      <c r="E26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="H26" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="J26" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B27" s="1">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
       </c>
       <c r="D27" s="2">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F27" s="3"/>
-      <c r="H27" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="I27" s="5" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B28" s="1">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
       </c>
       <c r="D28" s="2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F28" s="3"/>
       <c r="H28" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I28" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I28" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J28" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B29" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
       </c>
       <c r="D29" s="2">
-        <v>16</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>59</v>
+        <v>14</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="F29" s="3"/>
-      <c r="H29" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="I29" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B30" s="1">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
       </c>
       <c r="D30" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>61</v>
@@ -2001,21 +2029,21 @@
         <v>62</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
       </c>
       <c r="D31" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>63</v>
@@ -2025,7 +2053,7 @@
         <v>64</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -2039,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>65</v>
@@ -2049,220 +2077,199 @@
         <v>66</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
       </c>
       <c r="D33" s="2">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>67</v>
       </c>
       <c r="F33" s="3"/>
-      <c r="H33" s="8" t="s">
+      <c r="H33" s="4" t="s">
         <v>68</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B34" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
       </c>
       <c r="D34" s="2">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F34" s="3"/>
       <c r="H34" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
       </c>
       <c r="D35" s="2">
-        <v>20</v>
-      </c>
-      <c r="E35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="I35" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F35" s="3"/>
-      <c r="H35" s="8" t="s">
+    </row>
+    <row r="36" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>26</v>
+      </c>
+      <c r="B36" s="1">
+        <v>26</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="2">
+        <v>56</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I35" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>28</v>
-      </c>
-      <c r="B36" s="1">
-        <v>28</v>
-      </c>
-      <c r="C36" s="1">
-        <v>0</v>
-      </c>
-      <c r="D36" s="2">
-        <v>21</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="3"/>
+      <c r="H36" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="H36" s="8" t="s">
-        <v>75</v>
-      </c>
       <c r="I36" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C37" s="1">
         <v>0</v>
       </c>
       <c r="D37" s="2">
-        <v>22</v>
-      </c>
-      <c r="E37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="I37" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>28</v>
+      </c>
+      <c r="B38" s="1">
+        <v>28</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="2">
+        <v>21</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F37" s="3"/>
-      <c r="H37" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>30</v>
-      </c>
-      <c r="B38" s="1">
-        <v>30</v>
-      </c>
-      <c r="C38" s="1">
-        <v>0</v>
-      </c>
-      <c r="D38" s="2">
-        <v>23</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="F38" s="3"/>
-      <c r="H38" s="8" t="s">
-        <v>79</v>
-      </c>
       <c r="I38" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
       </c>
       <c r="D39" s="2">
-        <v>46</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>80</v>
+        <v>22</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="F39" s="3"/>
-      <c r="H39" s="4" t="s">
-        <v>81</v>
-      </c>
       <c r="I39" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C40" s="1">
         <v>0</v>
       </c>
       <c r="D40" s="2">
-        <v>48</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>82</v>
+        <v>23</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="F40" s="3"/>
-      <c r="H40" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="I40" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -2276,20 +2283,20 @@
         <v>0</v>
       </c>
       <c r="D41" s="2">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F41" s="3"/>
       <c r="H41" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -2303,20 +2310,20 @@
         <v>0</v>
       </c>
       <c r="D42" s="2">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F42" s="3"/>
       <c r="H42" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -2330,740 +2337,746 @@
         <v>0</v>
       </c>
       <c r="D43" s="2">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F43" s="3"/>
       <c r="H43" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>31</v>
+      </c>
+      <c r="B44" s="1">
+        <v>31</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2">
+        <v>51</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="H44" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>31</v>
+      </c>
+      <c r="B45" s="1">
+        <v>31</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="2">
+        <v>54</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45" s="3"/>
+      <c r="H45" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>32</v>
+      </c>
+      <c r="B46" s="1">
+        <v>32</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2">
+        <v>25</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I43" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J43" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
+      <c r="F46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
         <v>32</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B47" s="1">
         <v>32</v>
       </c>
-      <c r="C44" s="1">
-        <v>0</v>
-      </c>
-      <c r="D44" s="2">
-        <v>25</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F44" s="3" t="s">
+      <c r="C47" s="1">
+        <v>0</v>
+      </c>
+      <c r="D47" s="2">
         <v>91</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="E47" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="I47" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J47" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
-        <v>32</v>
-      </c>
-      <c r="B45" s="1">
-        <v>32</v>
-      </c>
-      <c r="C45" s="1">
-        <v>0</v>
-      </c>
-      <c r="D45" s="2">
-        <v>91</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F45" s="3"/>
-      <c r="I45" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
-        <v>33</v>
-      </c>
-      <c r="B46" s="1">
-        <v>33</v>
-      </c>
-      <c r="C46" s="1">
-        <v>0</v>
-      </c>
-      <c r="D46" s="2">
-        <v>26</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J46" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
-        <v>34</v>
-      </c>
-      <c r="B47" s="1">
-        <v>34</v>
-      </c>
-      <c r="C47" s="1">
-        <v>0</v>
-      </c>
-      <c r="D47" s="2">
-        <v>27</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B48" s="1">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C48" s="1">
         <v>0</v>
       </c>
       <c r="D48" s="2">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F48" s="3"/>
+        <v>94</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="I48" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J48" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
+        <v>34</v>
+      </c>
+      <c r="B49" s="1">
+        <v>34</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2">
+        <v>27</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>35</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B50" s="1">
         <v>35</v>
       </c>
-      <c r="C49" s="1">
-        <v>0</v>
-      </c>
-      <c r="D49" s="2">
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2">
+        <v>28</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F50" s="3"/>
+      <c r="I50" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>35</v>
+      </c>
+      <c r="B51" s="1">
+        <v>35</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0</v>
+      </c>
+      <c r="D51" s="2">
         <v>29</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F51" s="3"/>
+      <c r="I51" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>36</v>
+      </c>
+      <c r="B52" s="1">
+        <v>36</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0</v>
+      </c>
+      <c r="D52" s="2">
+        <v>30</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F49" s="3"/>
-      <c r="I49" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
-        <v>36</v>
-      </c>
-      <c r="B50" s="1">
-        <v>36</v>
-      </c>
-      <c r="C50" s="1">
-        <v>0</v>
-      </c>
-      <c r="D50" s="2">
-        <v>30</v>
-      </c>
-      <c r="E50" s="1" t="s">
+      <c r="F52" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>37</v>
-      </c>
-      <c r="B51" s="1">
-        <v>37</v>
-      </c>
-      <c r="C51" s="1">
-        <v>0</v>
-      </c>
-      <c r="D51" s="2">
-        <v>31</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>38</v>
-      </c>
-      <c r="B52" s="1">
-        <v>38</v>
-      </c>
-      <c r="C52" s="1">
-        <v>0</v>
-      </c>
-      <c r="D52" s="2">
-        <v>32</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F52" s="3"/>
       <c r="I52" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B53" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C53" s="1">
         <v>0</v>
       </c>
       <c r="D53" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I53" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J53" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="J53" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B54" s="1">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C54" s="1">
         <v>0</v>
       </c>
       <c r="D54" s="2">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F54" s="3"/>
       <c r="I54" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J54" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B55" s="1">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C55" s="1">
         <v>0</v>
       </c>
       <c r="D55" s="2">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F55" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="I55" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J55" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="J55" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B56" s="1">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C56" s="1">
         <v>0</v>
       </c>
       <c r="D56" s="2">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>112</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="F56" s="3"/>
       <c r="I56" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J56" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B57" s="1">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C57" s="1">
         <v>0</v>
       </c>
       <c r="D57" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F57" s="3"/>
       <c r="I57" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>42</v>
+      </c>
+      <c r="B58" s="1">
+        <v>42</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0</v>
+      </c>
+      <c r="D58" s="2">
+        <v>42</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>43</v>
+      </c>
+      <c r="B59" s="1">
+        <v>43</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0</v>
+      </c>
+      <c r="D59" s="2">
+        <v>36</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F59" s="3"/>
+      <c r="I59" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J59" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="J57" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
-        <v>44</v>
-      </c>
-      <c r="B58" s="1">
-        <v>44</v>
-      </c>
-      <c r="C58" s="1">
-        <v>0</v>
-      </c>
-      <c r="D58" s="2">
-        <v>37</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
-        <v>45</v>
-      </c>
-      <c r="B59" s="1">
-        <v>45</v>
-      </c>
-      <c r="C59" s="1">
-        <v>0</v>
-      </c>
-      <c r="D59" s="2">
-        <v>38</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="I59" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="J59" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
+        <v>44</v>
+      </c>
+      <c r="B60" s="1">
+        <v>44</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0</v>
+      </c>
+      <c r="D60" s="2">
+        <v>37</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
         <v>45</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B61" s="1">
         <v>45</v>
       </c>
-      <c r="C60" s="1">
-        <v>0</v>
-      </c>
-      <c r="D60" s="2">
+      <c r="C61" s="1">
+        <v>0</v>
+      </c>
+      <c r="D61" s="2">
+        <v>38</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>45</v>
+      </c>
+      <c r="B62" s="1">
+        <v>45</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0</v>
+      </c>
+      <c r="D62" s="2">
         <v>90</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="I62" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>46</v>
+      </c>
+      <c r="B63" s="1">
+        <v>46</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+      <c r="D63" s="2">
+        <v>75</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="I60" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="J60" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
-        <v>46</v>
-      </c>
-      <c r="B61" s="1">
-        <v>46</v>
-      </c>
-      <c r="C61" s="1">
-        <v>0</v>
-      </c>
-      <c r="D61" s="2">
-        <v>75</v>
-      </c>
-      <c r="E61" s="1" t="s">
+      <c r="F63" s="3"/>
+      <c r="I63" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J63" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="F61" s="3"/>
-      <c r="I61" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="J61" s="5" t="s">
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>47</v>
+      </c>
+      <c r="B64" s="1">
+        <v>47</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0</v>
+      </c>
+      <c r="D64" s="2">
+        <v>76</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
-        <v>47</v>
-      </c>
-      <c r="B62" s="1">
-        <v>47</v>
-      </c>
-      <c r="C62" s="1">
-        <v>0</v>
-      </c>
-      <c r="D62" s="2">
-        <v>76</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F62" s="3"/>
-      <c r="I62" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="J62" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
-        <v>48</v>
-      </c>
-      <c r="B63" s="1">
-        <v>48</v>
-      </c>
-      <c r="C63" s="1">
-        <v>0</v>
-      </c>
-      <c r="D63" s="2">
-        <v>77</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="51" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
-        <v>49</v>
-      </c>
-      <c r="B64" s="1">
-        <v>49</v>
-      </c>
-      <c r="C64" s="1">
-        <v>0</v>
-      </c>
-      <c r="D64" s="2">
-        <v>78</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="F64" s="3"/>
       <c r="I64" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>48</v>
+      </c>
+      <c r="B65" s="1">
+        <v>48</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+      <c r="D65" s="2">
+        <v>77</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>49</v>
+      </c>
+      <c r="B66" s="1">
+        <v>49</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0</v>
+      </c>
+      <c r="D66" s="2">
+        <v>78</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J64" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
-        <v>50</v>
-      </c>
-      <c r="B65" s="1">
-        <v>50</v>
-      </c>
-      <c r="C65" s="1">
-        <v>0</v>
-      </c>
-      <c r="D65" s="2">
-        <v>39</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
-        <v>51</v>
-      </c>
-      <c r="B66" s="1">
-        <v>51</v>
-      </c>
-      <c r="C66" s="1">
-        <v>0</v>
-      </c>
-      <c r="D66" s="2">
-        <v>40</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>136</v>
-      </c>
+      <c r="F66" s="3"/>
       <c r="I66" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
+        <v>50</v>
+      </c>
+      <c r="B67" s="1">
+        <v>50</v>
+      </c>
+      <c r="C67" s="1">
+        <v>0</v>
+      </c>
+      <c r="D67" s="2">
+        <v>39</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I67" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
         <v>51</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B68" s="1">
         <v>51</v>
       </c>
-      <c r="C67" s="1">
-        <v>0</v>
-      </c>
-      <c r="D67" s="2">
-        <v>89</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I67" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="J67" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
-        <v>52</v>
-      </c>
-      <c r="B68" s="1">
-        <v>52</v>
-      </c>
       <c r="C68" s="1">
         <v>0</v>
       </c>
       <c r="D68" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="I68" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B69" s="1">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C69" s="1">
         <v>0</v>
       </c>
       <c r="D69" s="2">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F69" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="I69" s="5" t="s">
-        <v>12</v>
+        <v>130</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B70" s="1">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C70" s="1">
         <v>0</v>
       </c>
       <c r="D70" s="2">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="F70" s="3"/>
+        <v>139</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="I70" s="5" t="s">
-        <v>12</v>
+        <v>130</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>21</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B71" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C71" s="1">
         <v>0</v>
       </c>
       <c r="D71" s="2">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F71" s="3"/>
       <c r="I71" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B72" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C72" s="1">
         <v>0</v>
       </c>
       <c r="D72" s="2">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F72" s="3"/>
       <c r="I72" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
@@ -3077,17 +3090,17 @@
         <v>0</v>
       </c>
       <c r="D73" s="2">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F73" s="3"/>
       <c r="I73" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
@@ -3101,199 +3114,205 @@
         <v>0</v>
       </c>
       <c r="D74" s="2">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F74" s="3"/>
       <c r="I74" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B75" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75" s="1">
         <v>0</v>
       </c>
       <c r="D75" s="2">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F75" s="3"/>
       <c r="I75" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J75" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B76" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C76" s="1">
         <v>0</v>
       </c>
       <c r="D76" s="2">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F76" s="3"/>
       <c r="I76" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B77" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C77" s="1">
         <v>0</v>
       </c>
       <c r="D77" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F77" s="3"/>
       <c r="I77" s="5" t="s">
-        <v>114</v>
+        <v>13</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B78" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C78" s="1">
         <v>0</v>
       </c>
       <c r="D78" s="2">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F78" s="3"/>
       <c r="I78" s="5" t="s">
-        <v>114</v>
+        <v>13</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B79" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C79" s="1">
         <v>0</v>
       </c>
       <c r="D79" s="2">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F79" s="3"/>
       <c r="I79" s="5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A80" s="2">
-        <v>61</v>
-      </c>
-      <c r="B80" s="2">
-        <v>8</v>
-      </c>
-      <c r="C80" s="2">
-        <v>1</v>
+        <v>113</v>
+      </c>
+      <c r="J79" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>59</v>
+      </c>
+      <c r="B80" s="1">
+        <v>6</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0</v>
       </c>
       <c r="D80" s="2">
-        <v>68</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F80" s="9"/>
+        <v>66</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F80" s="3"/>
       <c r="I80" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="J80" s="11"/>
-    </row>
-    <row r="81" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B81" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C81" s="1">
         <v>0</v>
       </c>
       <c r="D81" s="2">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F81" s="3"/>
       <c r="I81" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A82" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A82" s="2">
         <v>61</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="2">
         <v>8</v>
       </c>
-      <c r="C82" s="1">
-        <v>0</v>
+      <c r="C82" s="2">
+        <v>1</v>
       </c>
       <c r="D82" s="2">
-        <v>100</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F82" s="3"/>
+        <v>68</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F82" s="8"/>
       <c r="I82" s="5" t="s">
-        <v>131</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="J82" s="10"/>
     </row>
     <row r="83" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
@@ -3306,14 +3325,14 @@
         <v>0</v>
       </c>
       <c r="D83" s="2">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F83" s="3"/>
       <c r="I83" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3327,14 +3346,14 @@
         <v>0</v>
       </c>
       <c r="D84" s="2">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F84" s="3"/>
       <c r="I84" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3348,14 +3367,14 @@
         <v>0</v>
       </c>
       <c r="D85" s="2">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F85" s="3"/>
       <c r="I85" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3369,14 +3388,14 @@
         <v>0</v>
       </c>
       <c r="D86" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F86" s="3"/>
       <c r="I86" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3390,14 +3409,14 @@
         <v>0</v>
       </c>
       <c r="D87" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F87" s="3"/>
       <c r="I87" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3411,14 +3430,14 @@
         <v>0</v>
       </c>
       <c r="D88" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F88" s="3"/>
       <c r="I88" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
@@ -3432,79 +3451,79 @@
         <v>0</v>
       </c>
       <c r="D89" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F89" s="3"/>
       <c r="I89" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A90" s="2">
-        <v>62</v>
-      </c>
-      <c r="B90" s="2">
-        <v>9</v>
-      </c>
-      <c r="C90" s="2">
-        <v>1</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>61</v>
+      </c>
+      <c r="B90" s="1">
+        <v>8</v>
+      </c>
+      <c r="C90" s="1">
+        <v>0</v>
       </c>
       <c r="D90" s="2">
-        <v>69</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F90" s="9"/>
+        <v>106</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F90" s="3"/>
       <c r="I90" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="J90" s="11"/>
+        <v>130</v>
+      </c>
     </row>
     <row r="91" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B91" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C91" s="1">
         <v>0</v>
       </c>
       <c r="D91" s="2">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F91" s="3"/>
       <c r="I91" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A92" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A92" s="2">
         <v>62</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92" s="2">
         <v>9</v>
       </c>
-      <c r="C92" s="1">
-        <v>0</v>
+      <c r="C92" s="2">
+        <v>1</v>
       </c>
       <c r="D92" s="2">
-        <v>93</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="F92" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="F92" s="8"/>
       <c r="I92" s="5" t="s">
-        <v>131</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="J92" s="10"/>
     </row>
     <row r="93" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
@@ -3517,150 +3536,192 @@
         <v>0</v>
       </c>
       <c r="D93" s="2">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F93" s="3"/>
       <c r="I93" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A94" s="2">
-        <v>63</v>
-      </c>
-      <c r="B94" s="2">
-        <v>10</v>
-      </c>
-      <c r="C94" s="2">
-        <v>1</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>62</v>
+      </c>
+      <c r="B94" s="1">
+        <v>9</v>
+      </c>
+      <c r="C94" s="1">
+        <v>0</v>
       </c>
       <c r="D94" s="2">
-        <v>70</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F94" s="9"/>
+        <v>93</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F94" s="3"/>
       <c r="I94" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="J94" s="5" t="s">
-        <v>39</v>
+        <v>130</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B95" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C95" s="1">
         <v>0</v>
       </c>
       <c r="D95" s="2">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F95" s="3"/>
       <c r="I95" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="J95" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A96" s="1">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A96" s="2">
         <v>63</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96" s="2">
         <v>10</v>
       </c>
-      <c r="C96" s="1">
-        <v>0</v>
+      <c r="C96" s="2">
+        <v>1</v>
       </c>
       <c r="D96" s="2">
-        <v>96</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F96" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F96" s="8"/>
       <c r="I96" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A97" s="2">
-        <v>64</v>
-      </c>
-      <c r="B97" s="2">
-        <v>11</v>
-      </c>
-      <c r="C97" s="2">
-        <v>1</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>63</v>
+      </c>
+      <c r="B97" s="1">
+        <v>10</v>
+      </c>
+      <c r="C97" s="1">
+        <v>0</v>
       </c>
       <c r="D97" s="2">
-        <v>71</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F97" s="9"/>
+        <v>95</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F97" s="3"/>
       <c r="I97" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="J97" s="11"/>
+        <v>130</v>
+      </c>
+      <c r="J97" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="98" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B98" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C98" s="1">
         <v>0</v>
       </c>
       <c r="D98" s="2">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F98" s="3"/>
       <c r="I98" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A99" s="1">
+        <v>130</v>
+      </c>
+      <c r="J98" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" s="9" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A99" s="2">
         <v>64</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99" s="2">
         <v>11</v>
       </c>
-      <c r="C99" s="1">
-        <v>0</v>
+      <c r="C99" s="2">
+        <v>1</v>
       </c>
       <c r="D99" s="2">
+        <v>71</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F99" s="8"/>
+      <c r="I99" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J99" s="10"/>
+    </row>
+    <row r="100" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>64</v>
+      </c>
+      <c r="B100" s="1">
+        <v>11</v>
+      </c>
+      <c r="C100" s="1">
+        <v>0</v>
+      </c>
+      <c r="D100" s="2">
+        <v>97</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F100" s="3"/>
+      <c r="I100" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>64</v>
+      </c>
+      <c r="B101" s="1">
+        <v>11</v>
+      </c>
+      <c r="C101" s="1">
+        <v>0</v>
+      </c>
+      <c r="D101" s="2">
         <v>98</v>
       </c>
-      <c r="E99" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F99" s="3"/>
-      <c r="I99" s="5" t="s">
-        <v>131</v>
+      <c r="E101" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F101" s="3"/>
+      <c r="I101" s="5" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3675,7 +3736,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A2C1B7-577A-41EC-A9A3-19E5B67FC58E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DDB3C4-32A6-4E8C-B125-7A123899BE0C}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>